<commit_message>
updating interim model workout
</commit_message>
<xml_diff>
--- a/model/check.xlsx
+++ b/model/check.xlsx
@@ -468,20 +468,20 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>AMAT</t>
+          <t>AZO</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.1156476070299998</v>
+        <v>0.05971495234788682</v>
       </c>
       <c r="D2" t="n">
-        <v>94.74822188626848</v>
+        <v>2179.433870967742</v>
       </c>
       <c r="E2" t="n">
-        <v>107.1385373516851</v>
+        <v>2056.622741935484</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -490,20 +490,20 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>AMAT</t>
+          <t>AZO</t>
         </is>
       </c>
       <c r="B3" t="n">
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.004096959510413445</v>
+        <v>0.1105403963296181</v>
       </c>
       <c r="D3" t="n">
-        <v>94.36004225751677</v>
+        <v>2420.34935483871</v>
       </c>
       <c r="E3" t="n">
-        <v>94.74822188626848</v>
+        <v>2179.433870967742</v>
       </c>
       <c r="F3" t="n">
         <v>1</v>
@@ -512,20 +512,20 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>AMAT</t>
+          <t>AZO</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1977273158158825</v>
+        <v>0.007667381528366324</v>
       </c>
       <c r="D4" t="n">
-        <v>113.0176001333688</v>
+        <v>2438.907096774193</v>
       </c>
       <c r="E4" t="n">
-        <v>94.36004225751677</v>
+        <v>2420.34935483871</v>
       </c>
       <c r="F4" t="n">
         <v>2</v>
@@ -534,20 +534,20 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>AMAT</t>
+          <t>AZO</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>0.09262478206597469</v>
+        <v>0.04570489796328658</v>
       </c>
       <c r="D5" t="n">
-        <v>123.4858307153416</v>
+        <v>2550.377096774193</v>
       </c>
       <c r="E5" t="n">
-        <v>113.0176001333688</v>
+        <v>2438.907096774193</v>
       </c>
       <c r="F5" t="n">
         <v>3</v>
@@ -556,20 +556,20 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>AMAT</t>
+          <t>AZO</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1481423129662054</v>
+        <v>-0.01588493744568298</v>
       </c>
       <c r="D6" t="n">
-        <v>141.7793072960656</v>
+        <v>2509.864516129032</v>
       </c>
       <c r="E6" t="n">
-        <v>123.4858307153416</v>
+        <v>2550.377096774193</v>
       </c>
       <c r="F6" t="n">
         <v>4</v>
@@ -578,20 +578,20 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>CSCO</t>
+          <t>DPZ</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.0631398544076478</v>
+        <v>0.02734766921420384</v>
       </c>
       <c r="D7" t="n">
-        <v>41.09745613986918</v>
+        <v>366.6559349455675</v>
       </c>
       <c r="E7" t="n">
-        <v>43.86722642992176</v>
+        <v>356.8956702126114</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
@@ -600,20 +600,20 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>CSCO</t>
+          <t>DPZ</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>0.03521068928762983</v>
+        <v>-0.07257283276264426</v>
       </c>
       <c r="D8" t="n">
-        <v>42.54452589852211</v>
+        <v>340.0466750973318</v>
       </c>
       <c r="E8" t="n">
-        <v>41.09745613986918</v>
+        <v>366.6559349455675</v>
       </c>
       <c r="F8" t="n">
         <v>1</v>
@@ -622,20 +622,20 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>CSCO</t>
+          <t>DPZ</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>0.07977543201662263</v>
+        <v>-0.04669722367395546</v>
       </c>
       <c r="D9" t="n">
-        <v>45.9385338320191</v>
+        <v>324.1674394507269</v>
       </c>
       <c r="E9" t="n">
-        <v>42.54452589852211</v>
+        <v>340.0466750973318</v>
       </c>
       <c r="F9" t="n">
         <v>2</v>
@@ -644,20 +644,20 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>CSCO</t>
+          <t>DPZ</t>
         </is>
       </c>
       <c r="B10" t="n">
         <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>0.01478250260967595</v>
+        <v>-0.04820661875797649</v>
       </c>
       <c r="D10" t="n">
-        <v>46.61762032827561</v>
+        <v>308.5404232833762</v>
       </c>
       <c r="E10" t="n">
-        <v>45.9385338320191</v>
+        <v>324.1674394507269</v>
       </c>
       <c r="F10" t="n">
         <v>3</v>
@@ -666,20 +666,20 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>CSCO</t>
+          <t>DPZ</t>
         </is>
       </c>
       <c r="B11" t="n">
         <v>1</v>
       </c>
       <c r="C11" t="n">
-        <v>0.1060573503067628</v>
+        <v>0.2265847966660433</v>
       </c>
       <c r="D11" t="n">
-        <v>51.5617616178992</v>
+        <v>378.450992356295</v>
       </c>
       <c r="E11" t="n">
-        <v>46.61762032827561</v>
+        <v>308.5404232833762</v>
       </c>
       <c r="F11" t="n">
         <v>4</v>
@@ -688,20 +688,20 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>DHI</t>
+          <t>FICO</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>0.05131609404139992</v>
+        <v>0.1545034504137472</v>
       </c>
       <c r="D12" t="n">
-        <v>71.86762378505311</v>
+        <v>455.323870967742</v>
       </c>
       <c r="E12" t="n">
-        <v>68.35967240716761</v>
+        <v>394.3893548387097</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
@@ -710,20 +710,20 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>DHI</t>
+          <t>FICO</t>
         </is>
       </c>
       <c r="B13" t="n">
         <v>1</v>
       </c>
       <c r="C13" t="n">
-        <v>0.09264889853183411</v>
+        <v>0.1592521168909191</v>
       </c>
       <c r="D13" t="n">
-        <v>78.52607996883853</v>
+        <v>527.8351612903226</v>
       </c>
       <c r="E13" t="n">
-        <v>71.86762378505311</v>
+        <v>455.323870967742</v>
       </c>
       <c r="F13" t="n">
         <v>1</v>
@@ -732,20 +732,20 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>DHI</t>
+          <t>FICO</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>1</v>
       </c>
       <c r="C14" t="n">
-        <v>0.191510704660981</v>
+        <v>0.2602080072652202</v>
       </c>
       <c r="D14" t="n">
-        <v>93.56466487793534</v>
+        <v>665.1820967741936</v>
       </c>
       <c r="E14" t="n">
-        <v>78.52607996883853</v>
+        <v>527.8351612903226</v>
       </c>
       <c r="F14" t="n">
         <v>2</v>
@@ -754,20 +754,20 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>DHI</t>
+          <t>FICO</t>
         </is>
       </c>
       <c r="B15" t="n">
         <v>1</v>
       </c>
       <c r="C15" t="n">
-        <v>0.1495786539611208</v>
+        <v>0.1271790964831603</v>
       </c>
       <c r="D15" t="n">
-        <v>107.5599415087003</v>
+        <v>749.7793548387097</v>
       </c>
       <c r="E15" t="n">
-        <v>93.56466487793534</v>
+        <v>665.1820967741936</v>
       </c>
       <c r="F15" t="n">
         <v>3</v>
@@ -776,20 +776,20 @@
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>DHI</t>
+          <t>FICO</t>
         </is>
       </c>
       <c r="B16" t="n">
         <v>1</v>
       </c>
       <c r="C16" t="n">
-        <v>0.09705292814023436</v>
+        <v>0.1459713309205806</v>
       </c>
       <c r="D16" t="n">
-        <v>117.998948782712</v>
+        <v>859.2256451612903</v>
       </c>
       <c r="E16" t="n">
-        <v>107.5599415087003</v>
+        <v>749.7793548387097</v>
       </c>
       <c r="F16" t="n">
         <v>4</v>
@@ -798,20 +798,20 @@
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>NVDA</t>
+          <t>VRSN</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.160322970090198</v>
+        <v>0.01086814113459522</v>
       </c>
       <c r="D17" t="n">
-        <v>15.82442056149998</v>
+        <v>185.4240322580645</v>
       </c>
       <c r="E17" t="n">
-        <v>18.84584191043054</v>
+        <v>183.4304838709677</v>
       </c>
       <c r="F17" t="n">
         <v>0</v>
@@ -820,20 +820,20 @@
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>NVDA</t>
+          <t>VRSN</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.07190094923551016</v>
+        <v>0.03492083098112531</v>
       </c>
       <c r="D18" t="n">
-        <v>14.68662970202621</v>
+        <v>191.8991935483871</v>
       </c>
       <c r="E18" t="n">
-        <v>15.82442056149998</v>
+        <v>185.4240322580645</v>
       </c>
       <c r="F18" t="n">
         <v>1</v>
@@ -842,20 +842,20 @@
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>NVDA</t>
+          <t>VRSN</t>
         </is>
       </c>
       <c r="B19" t="n">
         <v>1</v>
       </c>
       <c r="C19" t="n">
-        <v>0.4724850906622908</v>
+        <v>0.07438549305540976</v>
       </c>
       <c r="D19" t="n">
-        <v>21.62584326831156</v>
+        <v>206.1737096774194</v>
       </c>
       <c r="E19" t="n">
-        <v>14.68662970202621</v>
+        <v>191.8991935483871</v>
       </c>
       <c r="F19" t="n">
         <v>2</v>
@@ -864,20 +864,20 @@
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>NVDA</t>
+          <t>VRSN</t>
         </is>
       </c>
       <c r="B20" t="n">
         <v>1</v>
       </c>
       <c r="C20" t="n">
-        <v>0.5343764445371393</v>
+        <v>0.06923460251573021</v>
       </c>
       <c r="D20" t="n">
-        <v>33.18218450414932</v>
+        <v>220.4480645161291</v>
       </c>
       <c r="E20" t="n">
-        <v>21.62584326831156</v>
+        <v>206.1737096774194</v>
       </c>
       <c r="F20" t="n">
         <v>3</v>
@@ -886,20 +886,20 @@
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>NVDA</t>
+          <t>VRSN</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21" t="n">
-        <v>0.3507423958194766</v>
+        <v>-0.0592283457884164</v>
       </c>
       <c r="D21" t="n">
-        <v>44.82058339565857</v>
+        <v>207.3912903225806</v>
       </c>
       <c r="E21" t="n">
-        <v>33.18218450414932</v>
+        <v>220.4480645161291</v>
       </c>
       <c r="F21" t="n">
         <v>4</v>
@@ -908,20 +908,20 @@
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>ULTA</t>
+          <t>WEC</t>
         </is>
       </c>
       <c r="B22" t="n">
         <v>1</v>
       </c>
       <c r="C22" t="n">
-        <v>0.0152858863792813</v>
+        <v>0.01539204956007412</v>
       </c>
       <c r="D22" t="n">
-        <v>403.4575806451613</v>
+        <v>93.1093123853353</v>
       </c>
       <c r="E22" t="n">
-        <v>397.3832258064516</v>
+        <v>91.69789385851068</v>
       </c>
       <c r="F22" t="n">
         <v>0</v>
@@ -930,20 +930,20 @@
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>ULTA</t>
+          <t>WEC</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C23" t="n">
-        <v>0.06990182043361481</v>
+        <v>-0.08907424299135891</v>
       </c>
       <c r="D23" t="n">
-        <v>431.66</v>
+        <v>84.8156708691656</v>
       </c>
       <c r="E23" t="n">
-        <v>403.4575806451613</v>
+        <v>93.1093123853353</v>
       </c>
       <c r="F23" t="n">
         <v>1</v>
@@ -952,20 +952,20 @@
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>ULTA</t>
+          <t>WEC</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24" t="n">
-        <v>0.1890189859701408</v>
+        <v>0.009653156076683933</v>
       </c>
       <c r="D24" t="n">
-        <v>513.251935483871</v>
+        <v>85.63440977781431</v>
       </c>
       <c r="E24" t="n">
-        <v>431.66</v>
+        <v>84.8156708691656</v>
       </c>
       <c r="F24" t="n">
         <v>2</v>
@@ -974,20 +974,20 @@
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>ULTA</t>
+          <t>WEC</t>
         </is>
       </c>
       <c r="B25" t="n">
         <v>0</v>
       </c>
       <c r="C25" t="n">
-        <v>-0.04562856950714644</v>
+        <v>0.006272987585292045</v>
       </c>
       <c r="D25" t="n">
-        <v>489.8329838709677</v>
+        <v>86.17159336722436</v>
       </c>
       <c r="E25" t="n">
-        <v>513.251935483871</v>
+        <v>85.63440977781431</v>
       </c>
       <c r="F25" t="n">
         <v>3</v>
@@ -996,20 +996,20 @@
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>ULTA</t>
+          <t>WEC</t>
         </is>
       </c>
       <c r="B26" t="n">
         <v>0</v>
       </c>
       <c r="C26" t="n">
-        <v>-0.1088598500245886</v>
+        <v>-0.05177910667074004</v>
       </c>
       <c r="D26" t="n">
-        <v>436.5098387096774</v>
+        <v>81.70970524227522</v>
       </c>
       <c r="E26" t="n">
-        <v>489.8329838709677</v>
+        <v>86.17159336722436</v>
       </c>
       <c r="F26" t="n">
         <v>4</v>

</xml_diff>